<commit_message>
Alterações no Product backlog
</commit_message>
<xml_diff>
--- a/SPRINT2/PBC - Product Backlog Classified V2.xlsx
+++ b/SPRINT2/PBC - Product Backlog Classified V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\SPRINT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBBD344-3A01-491A-9F7F-A211F1D06B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8749434A-3DD8-4284-BDF8-392382EAD981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -557,14 +557,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -847,15 +839,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -882,9 +865,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="4" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -893,6 +873,18 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="21" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -919,196 +911,7 @@
     <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2525,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2544,37 +2347,37 @@
   <sheetData>
     <row r="1" spans="2:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:8" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="2:8" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" s="25" customFormat="1" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="36" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3030,75 +2833,75 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B5:E5 C5:C6 B6:B34">
-    <cfRule type="expression" dxfId="47" priority="34">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="35">
+    <cfRule type="expression" dxfId="19" priority="35">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="36">
+    <cfRule type="expression" dxfId="18" priority="36">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="37">
+    <cfRule type="expression" dxfId="17" priority="37">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="43" priority="26">
+    <cfRule type="expression" dxfId="16" priority="26">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="27">
+    <cfRule type="expression" dxfId="15" priority="27">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="28">
+    <cfRule type="expression" dxfId="14" priority="28">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="29">
+    <cfRule type="expression" dxfId="13" priority="29">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:E6">
-    <cfRule type="expression" dxfId="39" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="19">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="21">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C34">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D34">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$B8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$B8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>$B8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$B8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3134,387 +2937,387 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F378867A-5387-429E-B87E-19913A3BDAD1}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.44140625" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="41" customWidth="1"/>
-    <col min="4" max="14" width="8.88671875" style="41"/>
-    <col min="15" max="15" width="21.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="41"/>
+    <col min="1" max="1" width="34.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" style="38" customWidth="1"/>
+    <col min="4" max="14" width="8.88671875" style="38"/>
+    <col min="15" max="15" width="21.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="40"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="O2" s="41" t="s">
+      <c r="C2" s="40"/>
+      <c r="O2" s="38" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="O3" s="44" t="s">
+      <c r="C3" s="40"/>
+      <c r="O3" s="41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="40"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="40"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="40"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="40"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="40"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="40"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="40"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="43"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="40"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="43"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="43"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="43"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="40"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="42"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="43"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="40"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="43"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="43"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="40"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="43"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="40"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="43"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="40"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="43"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="40"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="43"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="40"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="42"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="43"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="40"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="42"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="43"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="40"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="42"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="43"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="40"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="42"/>
-      <c r="B51" s="42"/>
-      <c r="C51" s="43"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="40"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="42"/>
-      <c r="C52" s="43"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="42"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="43"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="40"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="42"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="43"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="42"/>
-      <c r="B55" s="42"/>
-      <c r="C55" s="43"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="40"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="42"/>
-      <c r="B56" s="42"/>
-      <c r="C56" s="43"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="40"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="42"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="43"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="40"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="42"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="43"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="40"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="42"/>
-      <c r="B59" s="42"/>
-      <c r="C59" s="43"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="40"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="42"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="43"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="40"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="42"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="43"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="40"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="PBC!A1" display="Tarefa principal" xr:uid="{D67C691F-7218-4113-A8E1-9129BD020CA5}"/>
-    <hyperlink ref="B1" location="PBC!A1" display="Descrição da tarefa" xr:uid="{77C0DF93-E2B8-4305-8DD0-5DF026725A24}"/>
+    <hyperlink ref="A1" location="PBC!A1" tooltip="Artefato de Referência (XX#R)" display="Tarefa principal" xr:uid="{D67C691F-7218-4113-A8E1-9129BD020CA5}"/>
+    <hyperlink ref="B1" location="PBC!A1" tooltip="Descrição do Requisito" display="Descrição da tarefa" xr:uid="{77C0DF93-E2B8-4305-8DD0-5DF026725A24}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3524,9 +3327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3537,10 +3338,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>